<commit_message>
Redistribucion de la Relacion Club-Membresia
</commit_message>
<xml_diff>
--- a/docs/DDL Bases de Datos/INSERTS.xlsx
+++ b/docs/DDL Bases de Datos/INSERTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1731c19597d6e0/Documents/GitHub/bases-uno/docs/DDL Bases de Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{E204D3BB-9F4C-4EA6-82BB-D9B58CA77049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF4EBF5A-757F-43AA-86B6-7335FBE61CD3}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="8_{E204D3BB-9F4C-4EA6-82BB-D9B58CA77049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DE99E00-8223-40B1-976C-12A1B274CCD7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="182">
   <si>
     <t>titulo</t>
   </si>
@@ -907,6 +907,180 @@
   </si>
   <si>
     <t>'Tails flies over Metropolis Zone in the Tornado, radioing Sonic. He says that all is quiet above, but Sonic has to fight his way through Badniks on the ground. Sonic figures he can handle things, but as reinforcements arrive, he reflects on how he d told his new friends Sally Acorn, Antoine Depardieu and Boomer Walrusâ€”to stay behind for their own safety. Now, he admits, he wouldn t mind their company.’</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>lugar_id</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>fecha_fundacion</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>pagina_web</t>
+  </si>
+  <si>
+    <t>proposito</t>
+  </si>
+  <si>
+    <t>membresia_coleccionista_documento_identidad</t>
+  </si>
+  <si>
+    <t>membresia_club_id</t>
+  </si>
+  <si>
+    <t>membresia_fecha_ingreso</t>
+  </si>
+  <si>
+    <t>documento_identidad</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>fecha_nacimiento</t>
+  </si>
+  <si>
+    <t>primer_nombre</t>
+  </si>
+  <si>
+    <t>segundo_nombre</t>
+  </si>
+  <si>
+    <t>primer_apellido</t>
+  </si>
+  <si>
+    <t>segundo_apellido</t>
+  </si>
+  <si>
+    <t>lugar_id_nacionalidad</t>
+  </si>
+  <si>
+    <t>coleccionista_documento_identidad</t>
+  </si>
+  <si>
+    <t>representante_documento_identidad</t>
+  </si>
+  <si>
+    <t>Alguno o Ambos es Null</t>
+  </si>
+  <si>
+    <t>lugar_id_direccion</t>
+  </si>
+  <si>
+    <t>usuario_email</t>
+  </si>
+  <si>
+    <t>plataforma</t>
+  </si>
+  <si>
+    <t>club_id</t>
+  </si>
+  <si>
+    <t>descripcion_detallada</t>
+  </si>
+  <si>
+    <t>fecha_registro</t>
+  </si>
+  <si>
+    <t>significado</t>
+  </si>
+  <si>
+    <t>coleccionable_id</t>
+  </si>
+  <si>
+    <t>precio_dolar</t>
+  </si>
+  <si>
+    <t>comic_id</t>
+  </si>
+  <si>
+    <t>O uno o el otro es null</t>
+  </si>
+  <si>
+    <t>nullable</t>
+  </si>
+  <si>
+    <t>alquilado</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>fecha_retiro</t>
+  </si>
+  <si>
+    <t>club_id_lider</t>
+  </si>
+  <si>
+    <t>email_contacto</t>
+  </si>
+  <si>
+    <t>mision</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>hora_inicio</t>
+  </si>
+  <si>
+    <t>hora_cierre</t>
+  </si>
+  <si>
+    <t>caridad</t>
+  </si>
+  <si>
+    <t>cancelado</t>
+  </si>
+  <si>
+    <t>local_id</t>
+  </si>
+  <si>
+    <t>id_inscripcion</t>
+  </si>
+  <si>
+    <t>subasta_id</t>
+  </si>
+  <si>
+    <t>autorizado</t>
+  </si>
+  <si>
+    <t>orden</t>
+  </si>
+  <si>
+    <t>precio_base_dolar</t>
+  </si>
+  <si>
+    <t>precio_vendido_dolar</t>
+  </si>
+  <si>
+    <t>dueno_historico_coleccionista_documento_identidad</t>
+  </si>
+  <si>
+    <t>dueno_historico_fecha_registro</t>
+  </si>
+  <si>
+    <t>participante_subasta_id</t>
+  </si>
+  <si>
+    <t>dueno_historico_id</t>
+  </si>
+  <si>
+    <t>participante_id_inscripcion</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,6 +1160,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1454,145 +1631,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63C948F-9E08-4D40-B549-C9CB75E908A0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DB7D4A-6BC3-495D-880B-C2E16F514A08}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F90F0B-2B22-4AE1-A94D-D0FA0E9EA9E3}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B29037-E2F2-4DD6-8FA5-A91D83ED3C0D}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8FCF63-23F5-49B7-80A5-F2DB7E22066C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0349695A-AC34-411A-BB82-EF82E7A55DC6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A6:A32"/>
+  <dimension ref="A2:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="6" spans="1:1">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1676,98 +2086,255 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:11">
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:11">
+      <c r="B4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="5" spans="1:11">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:11">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:11">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="8" spans="1:11">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC9179F-C46A-4456-9421-5B5AD8E0E34C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1776,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
@@ -1791,7 +2358,7 @@
     <col min="7" max="7" width="66.5703125" style="4" customWidth="1"/>
     <col min="8" max="9" width="11.5703125" style="4"/>
     <col min="10" max="10" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="63.85546875" style="4" customWidth="1"/>
     <col min="12" max="12" width="54.85546875" style="4" customWidth="1"/>
     <col min="13" max="13" width="64.42578125" style="4" customWidth="1"/>
     <col min="14" max="16384" width="11.5703125" style="4"/>
@@ -2127,7 +2694,7 @@
         <v>58</v>
       </c>
       <c r="K9" s="4" t="str">
-        <f t="shared" ref="K9:K65" si="1">IF(E9="null",_xlfn.CONCAT(L9," (",A8,"(",A9,",",B9,",",C9,",",D9,",",F9,",",G9,",",H9,",",I9,",",J9,");",),_xlfn.CONCAT(L9," (",A8,"(",A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,",",J9,");",))</f>
+        <f t="shared" ref="K9:K32" si="1">IF(E9="null",_xlfn.CONCAT(L9," (",A8,"(",A9,",",B9,",",C9,",",D9,",",F9,",",G9,",",H9,",",I9,",",J9,");",),_xlfn.CONCAT(L9," (",A8,"(",A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,",",J9,");",))</f>
         <v>INSERT INTO public.comic (titulo, volumen, numero, fecha_publicacion, precio_publicacion, color, sinopsis, paginas, cubierta, editor)  ('Tekken Comic’(‘Borderlands: Origins’,2,6, '11/15/2005’,31,TRUE,'The Last Voyage of the Infinite Succor takes place during the video game Halo: Combat Evolved. The Covenant Special Operations Commander Rtas ''Vadumee and his team are sent to answer the distress call from a Covenant agricultural ship, Infinite Succor. Believing that it might have been attacked by humans, ''Vadumee and his team instead discover the ship has been infested by the parasitic Flood, who gain the knowledge of those they infect and are trying to use the ship to escape imprisonment. Fighting waves of Flood, including the reanimated remains of his fallen soldiers, ''Vadumee plots a slipspace course that will destroy both Infinite Succor and the Flood, then escapes via a Covenant shuttle. ',41,TRUE,'Agustin Padilla’);</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -2683,7 +3250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="51">
+    <row r="23" spans="1:13" ht="21.75" customHeight="1">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -3118,12 +3685,60 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5946D3-6CF2-4DE6-B6A8-B706BEC7B812}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actuaizacion de Listado en CREATE e INSERT
</commit_message>
<xml_diff>
--- a/docs/DDL Bases de Datos/INSERTS.xlsx
+++ b/docs/DDL Bases de Datos/INSERTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1731c19597d6e0/Documents/GitHub/bases-uno/docs/DDL Bases de Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1901" documentId="8_{E204D3BB-9F4C-4EA6-82BB-D9B58CA77049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F102CE4-6B4B-4530-A17D-93D41F9F46F5}"/>
+  <xr:revisionPtr revIDLastSave="1917" documentId="8_{E204D3BB-9F4C-4EA6-82BB-D9B58CA77049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E0E739-2996-45D3-9505-B0E459981C74}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="695" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="695" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="605">
   <si>
     <t>titulo</t>
   </si>
@@ -1882,9 +1882,6 @@
     <t>INSERT INTO participante (id_inscripcion, subasta_id, membresia_coleccionista_documento_identidad, membresia_club_id, membresia_fecha_ingreso, autorizado) VALUES (</t>
   </si>
   <si>
-    <t>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (</t>
-  </si>
-  <si>
     <t>'1000'</t>
   </si>
   <si>
@@ -1931,6 +1928,18 @@
   </si>
   <si>
     <t>'2101'</t>
+  </si>
+  <si>
+    <t>duracion_min</t>
+  </si>
+  <si>
+    <t>'265'</t>
+  </si>
+  <si>
+    <t>'280'</t>
+  </si>
+  <si>
+    <t>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2037,6 +2046,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4222,7 +4234,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4662,7 +4674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C93953-163C-4729-8A74-95CB19FE497B}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -4678,13 +4690,13 @@
   <sheetData>
     <row r="2" spans="1:6" ht="20.25" thickBot="1">
       <c r="A2" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>153</v>
@@ -4698,7 +4710,7 @@
         <v>193</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>190</v>
@@ -4711,7 +4723,7 @@
         <v>INSERT INTO org_sub (porcentaje, monto_recibido, organizacion_caridad_id, subasta_is) VALUES ('10', '2101', '9', '9');</v>
       </c>
       <c r="F3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4971,10 +4983,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0349695A-AC34-411A-BB82-EF82E7A55DC6}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4989,11 +5001,12 @@
     <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="228.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="217" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" customWidth="1"/>
+    <col min="12" max="12" width="255.5703125" customWidth="1"/>
+    <col min="13" max="13" width="229.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
         <v>140</v>
       </c>
@@ -5004,7 +5017,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.25" thickBot="1">
+    <row r="2" spans="1:13" ht="20.25" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>107</v>
       </c>
@@ -5035,11 +5048,14 @@
       <c r="J2" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13.5" thickTop="1">
+    <row r="3" spans="1:13" ht="13.5" thickTop="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5050,7 +5066,7 @@
         <v>258</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>190</v>
@@ -5070,15 +5086,18 @@
       <c r="J3" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K3" t="str">
-        <f>_xlfn.CONCAT(L3,A3,", ",B3,", ",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,");",)</f>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (1, '1', '30', '60', '9', '1', '25385914', '3/3/2010', '2', '9');</v>
-      </c>
-      <c r="L3" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="K3" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L3" t="str">
+        <f>_xlfn.CONCAT(M3,A3,", ",B3,", ",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,");",)</f>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (1, '1', '30', '60', '9', '1', '25385914', '3/3/2010', '2', '9', '265');</v>
+      </c>
+      <c r="M3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5109,15 +5128,18 @@
       <c r="J4" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" ref="K4:K9" si="0">_xlfn.CONCAT(L4,A4,", ",B4,", ",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,");",)</f>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (2, '2', '800', '950', '9', '14', '25385914', '3/3/2010', '4', '9');</v>
-      </c>
-      <c r="L4" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="K4" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L11" si="0">_xlfn.CONCAT(M4,A4,", ",B4,", ",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,", ",K4,");",)</f>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (2, '2', '800', '950', '9', '14', '25385914', '3/3/2010', '4', '9', '265');</v>
+      </c>
+      <c r="M4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5125,10 +5147,10 @@
         <v>178</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>190</v>
@@ -5148,15 +5170,18 @@
       <c r="J5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (3, '3', '6500', '8500', '9', '27', '25385914', '3/3/2010', '5', '9');</v>
-      </c>
-      <c r="L5" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="K5" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (3, '3', '6500', '8500', '9', '27', '25385914', '3/3/2010', '5', '9', '265');</v>
+      </c>
+      <c r="M5" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5164,7 +5189,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>166</v>
@@ -5187,15 +5212,18 @@
       <c r="J6" t="s">
         <v>166</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (4, '4', '10000', NULL, '9', '10', '1998456', '3/3/2010', NULL, NULL);</v>
-      </c>
-      <c r="L6" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="K6" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (4, '4', '10000', NULL, '9', '10', '1998456', '3/3/2010', NULL, NULL, '265');</v>
+      </c>
+      <c r="M6" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5203,10 +5231,10 @@
         <v>176</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>190</v>
@@ -5226,15 +5254,18 @@
       <c r="J7" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (5, '5', '8600', '9000', '9', '23', '1998456', '3/3/2010', '4', '9');</v>
-      </c>
-      <c r="L7" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="K7" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (5, '5', '8600', '9000', '9', '23', '1998456', '3/3/2010', '4', '9', '265');</v>
+      </c>
+      <c r="M7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5242,7 +5273,7 @@
         <v>180</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>166</v>
@@ -5265,15 +5296,18 @@
       <c r="J8" t="s">
         <v>166</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (6, '6', '8600', NULL, '9', '36', '1998456', '3/3/2010', NULL, NULL);</v>
-      </c>
-      <c r="L8" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="K8" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (6, '6', '8600', NULL, '9', '36', '1998456', '3/3/2010', NULL, NULL, '265');</v>
+      </c>
+      <c r="M8" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5284,7 +5318,7 @@
         <v>515</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>190</v>
@@ -5304,15 +5338,18 @@
       <c r="J9" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (7, '7', '950', '1200', '9', '6', '1234567', '3/3/2010', '1', '9');</v>
-      </c>
-      <c r="L9" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="K9" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (7, '7', '950', '1200', '9', '6', '1234567', '3/3/2010', '1', '9', '265');</v>
+      </c>
+      <c r="M9" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5320,10 +5357,10 @@
         <v>188</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>190</v>
@@ -5343,15 +5380,18 @@
       <c r="J10" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" ref="K10:K21" si="1">_xlfn.CONCAT(L10,A10,", ",B10,", ",C10,", ",D10,", ",E10,", ",F10,", ",G10,", ",H10,", ",I10,", ",J10,");",)</f>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (8, '8', '150', '300', '9', '19', '1234567', '3/3/2010', '2', '9');</v>
-      </c>
-      <c r="L10" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="K10" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (8, '8', '150', '300', '9', '19', '1234567', '3/3/2010', '2', '9', '265');</v>
+      </c>
+      <c r="M10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5362,7 +5402,7 @@
         <v>515</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>190</v>
@@ -5382,12 +5422,15 @@
       <c r="J11" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="K11" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion) VALUES (9, '9', '950', '1000', '9', '32', '1234567', '3/3/2010', '5', '9');</v>
-      </c>
-      <c r="L11" t="s">
-        <v>585</v>
+      <c r="K11" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO listado (orden, precio_base_dolar, precio_vendido_dolar, subasta_id, dueno_historico_id, dueno_historico_coleccionista_documento_identidad, dueno_historico_fecha_registro, participante_subasta_id, participante_id_inscripcion, duracion_min) VALUES (9, '9', '950', '1000', '9', '32', '1234567', '3/3/2010', '5', '9', '280');</v>
+      </c>
+      <c r="M11" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -5434,6 +5477,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7391,7 +7435,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>472</v>
@@ -10510,10 +10554,10 @@
         <v>166</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" ref="H58:H74" si="1">_xlfn.CONCAT(I58, B58, ", ",C58, ", ",D58, ", ",E58, ", ",F58, ", ",G58, ");")</f>
+        <f t="shared" ref="H58:H64" si="1">_xlfn.CONCAT(I58, B58, ", ",C58, ", ",D58, ", ",E58, ", ",F58, ", ",G58, ");")</f>
         <v>INSERT INTO dueno_historico (fecha_registro, significado, coleccionista_documento_identidad, coleccionable_id, comic_id, precio_dolar) VALUES ('1/1/2019', NULL, '1998456', '1', NULL, '60');</v>
       </c>
       <c r="I58" t="s">
@@ -10570,7 +10614,7 @@
         <v>177</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
@@ -10600,7 +10644,7 @@
         <v>166</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="1"/>
@@ -10630,7 +10674,7 @@
         <v>166</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
@@ -10660,7 +10704,7 @@
         <v>166</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="1"/>
@@ -10690,7 +10734,7 @@
         <v>187</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>

</xml_diff>